<commit_message>
pandas excel loading and xlsx fixes
</commit_message>
<xml_diff>
--- a/Task 2/pozyxAPI_dane_pomiarowe/pozyxAPI_only_localization_measurement2.xlsx
+++ b/Task 2/pozyxAPI_dane_pomiarowe/pozyxAPI_only_localization_measurement2.xlsx
@@ -1,20 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciej Pracucik\Desktop\Repo\SISE\Task 2\pozyxAPI_dane_pomiarowe\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8E5422-BD0B-4814-9931-CDBA252C0212}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="4110" yWindow="1665" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="measurement" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>0/timestamp</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>measurement x</t>
+  </si>
+  <si>
+    <t>measurement y</t>
+  </si>
+  <si>
+    <t>reference x</t>
+  </si>
+  <si>
+    <t>reference y</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -532,24 +572,24 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - akcent 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - akcent 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - akcent 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - akcent 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - akcent 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - akcent 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - akcent 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - akcent 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - akcent 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - akcent 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - akcent 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - akcent 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - akcent 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - akcent 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - akcent 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - akcent 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - akcent 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Akcent 1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Akcent 2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Akcent 3" xfId="26" builtinId="37" customBuiltin="1"/>
@@ -558,14 +598,14 @@
     <cellStyle name="Akcent 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Dane wejściowe" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Dane wyjściowe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Dobre" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Dobry" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Komórka połączona" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Komórka zaznaczona" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Nagłówek 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Nagłówek 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Nagłówek 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Nagłówek 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Neutralne" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutralny" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
     <cellStyle name="Obliczenia" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Suma" xfId="17" builtinId="25" customBuiltin="1"/>
@@ -573,13 +613,16 @@
     <cellStyle name="Tekst ostrzeżenia" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Tytuł" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Uwaga" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Złe" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Zły" xfId="7" builtinId="27" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -628,7 +671,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -661,9 +704,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -696,6 +756,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -871,11 +948,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H1541"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -891,8 +968,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -2867,7 +2963,7 @@
       </c>
       <c r="C84" s="2">
         <f t="shared" si="1"/>
-        <v>5.2919998168945312</v>
+        <v>5.2919998168945313</v>
       </c>
       <c r="D84" s="4">
         <v>82</v>
@@ -4619,7 +4715,7 @@
       </c>
       <c r="C157" s="2">
         <f t="shared" si="2"/>
-        <v>10.277999877929687</v>
+        <v>10.277999877929688</v>
       </c>
       <c r="D157" s="4">
         <v>155</v>
@@ -10931,7 +11027,7 @@
       </c>
       <c r="C420" s="2">
         <f t="shared" si="6"/>
-        <v>29.277999877929687</v>
+        <v>29.277999877929688</v>
       </c>
       <c r="D420" s="4">
         <v>418</v>

</xml_diff>